<commit_message>
replace the running table excel and sorts.h
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -8,13 +8,107 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhanpengtong/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E6E959D-C983-A140-8126-F3D351C8ECBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265961B0-67B6-594E-91EE-35BFBEA86895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10900" yWindow="7140" windowWidth="28040" windowHeight="17440" xr2:uid="{243C1552-399E-D845-AF91-2DE6174E8523}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$B$1:$F$1</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$B$2:$F$2</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$B$3:$F$3</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$B$4:$F$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$B$5:$F$5</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$B$6:$F$6</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v2.30" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v2.31" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v2.32" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v2.33" hidden="1">Sheet1!$C$2:$C$6</definedName>
+    <definedName name="_xlchart.v2.34" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v2.35" hidden="1">Sheet1!$D$2:$D$6</definedName>
+    <definedName name="_xlchart.v2.36" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v2.37" hidden="1">Sheet1!$E$2:$E$6</definedName>
+    <definedName name="_xlchart.v2.38" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v2.39" hidden="1">Sheet1!$F$2:$F$6</definedName>
+    <definedName name="_xlchart.v2.40" hidden="1">Sheet1!$B$1:$F$1</definedName>
+    <definedName name="_xlchart.v2.41" hidden="1">Sheet1!$B$2:$F$2</definedName>
+    <definedName name="_xlchart.v2.42" hidden="1">Sheet1!$B$3:$F$3</definedName>
+    <definedName name="_xlchart.v2.43" hidden="1">Sheet1!$B$4:$F$4</definedName>
+    <definedName name="_xlchart.v2.44" hidden="1">Sheet1!$B$5:$F$5</definedName>
+    <definedName name="_xlchart.v2.45" hidden="1">Sheet1!$B$6:$F$6</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,14 +155,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,10 +195,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -113,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,15 +513,15 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F12" sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>10</v>
       </c>
@@ -460,7 +561,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>100</v>
       </c>
@@ -480,7 +581,7 @@
         <v>3.4E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -500,7 +601,7 @@
         <v>4.6900000000000002E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -520,7 +621,7 @@
         <v>1.9910000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10000</v>
       </c>
@@ -540,7 +641,7 @@
         <v>4.2129999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>50000</v>
       </c>
@@ -560,7 +661,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>100000</v>
       </c>
@@ -580,7 +681,7 @@
         <v>3.5707999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>125000</v>
       </c>
@@ -600,7 +701,7 @@
         <v>4.6143999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>150000</v>
       </c>
@@ -620,7 +721,7 @@
         <v>5.4782999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>175000</v>
       </c>
@@ -640,7 +741,7 @@
         <v>5.4969999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>200000</v>
       </c>
@@ -661,6 +762,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>